<commit_message>
Adiciona e atualiza regex, nlp mais robusto e correção de bugs do regex
</commit_message>
<xml_diff>
--- a/AMOSTRA_e-SIC.xlsx
+++ b/AMOSTRA_e-SIC.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="8_{E138E9C0-4016-468F-B21F-6ED2EC3A7584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E658EBA6-D54B-420F-B40B-1736D80A17F3}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17475" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amostra - SIC" sheetId="1" r:id="rId1"/>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="B60" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>